<commit_message>
edit to differentiate dermis according to apex distance from litterature
</commit_message>
<xml_diff>
--- a/simulations/inputs/Scenarios_24_06.xlsx
+++ b/simulations/inputs/Scenarios_24_06.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tigerault\package\Wheat-BRIDGES\Root_BRIDGES\root_cynaps\simulations\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAEB1F59-EDF1-47B2-B8AF-3637103FB0BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAC8CB72-B9E4-4F81-8C3E-B5E48D32C802}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,6 +17,7 @@
     <sheet name="Comparison_with_parameters.py" sheetId="4" state="hidden" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -2872,9 +2873,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N219"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="89" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="F1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="I11" sqref="I11"/>
+    <sheetView tabSelected="1" topLeftCell="A102" zoomScale="89" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="E1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="I108" sqref="I108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7538,28 +7539,28 @@
         <v>1</v>
       </c>
       <c r="I106" s="58">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <f>10/0.1</f>
+        <v>100</v>
       </c>
       <c r="J106" s="58">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <f t="shared" ref="J106:N106" si="1">10/0.1</f>
+        <v>100</v>
       </c>
       <c r="K106" s="58">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <f t="shared" si="1"/>
+        <v>100</v>
       </c>
       <c r="L106" s="58">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <f t="shared" si="1"/>
+        <v>100</v>
       </c>
       <c r="M106" s="58">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <f t="shared" si="1"/>
+        <v>100</v>
       </c>
       <c r="N106" s="58">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <f t="shared" si="1"/>
+        <v>100</v>
       </c>
     </row>
     <row r="107" spans="1:14" x14ac:dyDescent="0.3">
@@ -7586,32 +7587,32 @@
         <v>3</v>
       </c>
       <c r="H107" s="58">
-        <f t="shared" ref="H107:N107" si="1">150*H104</f>
+        <f t="shared" ref="H107:N107" si="2">150*H104</f>
         <v>150</v>
       </c>
       <c r="I107" s="58">
-        <f t="shared" si="1"/>
-        <v>150</v>
+        <f>150/0.1</f>
+        <v>1500</v>
       </c>
       <c r="J107" s="58">
-        <f t="shared" si="1"/>
-        <v>150</v>
+        <f t="shared" ref="J107:N107" si="3">150/0.1</f>
+        <v>1500</v>
       </c>
       <c r="K107" s="58">
-        <f t="shared" si="1"/>
-        <v>150</v>
+        <f t="shared" si="3"/>
+        <v>1500</v>
       </c>
       <c r="L107" s="58">
-        <f t="shared" si="1"/>
-        <v>150</v>
+        <f t="shared" si="3"/>
+        <v>1500</v>
       </c>
       <c r="M107" s="58">
-        <f t="shared" si="1"/>
-        <v>150</v>
+        <f t="shared" si="3"/>
+        <v>1500</v>
       </c>
       <c r="N107" s="58">
-        <f t="shared" si="1"/>
-        <v>150</v>
+        <f t="shared" si="3"/>
+        <v>1500</v>
       </c>
     </row>
     <row r="108" spans="1:14" x14ac:dyDescent="0.3">
@@ -7634,36 +7635,36 @@
         <v>506</v>
       </c>
       <c r="G108" s="58">
-        <f t="shared" ref="G108:N108" si="2">G99</f>
+        <f t="shared" ref="G108:N108" si="4">G99</f>
         <v>21</v>
       </c>
       <c r="H108" s="58">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>21</v>
       </c>
       <c r="I108" s="58">
-        <f t="shared" si="2"/>
-        <v>21</v>
+        <f>20/0.1</f>
+        <v>200</v>
       </c>
       <c r="J108" s="58">
-        <f t="shared" si="2"/>
-        <v>21</v>
+        <f t="shared" ref="J108:N108" si="5">20/0.1</f>
+        <v>200</v>
       </c>
       <c r="K108" s="58">
-        <f t="shared" si="2"/>
-        <v>21</v>
+        <f t="shared" si="5"/>
+        <v>200</v>
       </c>
       <c r="L108" s="58">
-        <f t="shared" si="2"/>
-        <v>21</v>
+        <f t="shared" si="5"/>
+        <v>200</v>
       </c>
       <c r="M108" s="58">
-        <f t="shared" si="2"/>
-        <v>21</v>
+        <f t="shared" si="5"/>
+        <v>200</v>
       </c>
       <c r="N108" s="58">
-        <f t="shared" si="2"/>
-        <v>21</v>
+        <f t="shared" si="5"/>
+        <v>200</v>
       </c>
     </row>
     <row r="109" spans="1:14" x14ac:dyDescent="0.3">
@@ -7690,32 +7691,32 @@
         <v>210</v>
       </c>
       <c r="H109" s="58">
-        <f t="shared" ref="H109:N109" si="3">70*H99</f>
+        <f t="shared" ref="H109:N109" si="6">70*H99</f>
         <v>1470</v>
       </c>
       <c r="I109" s="58">
-        <f t="shared" si="3"/>
-        <v>1470</v>
+        <f>400/0.1</f>
+        <v>4000</v>
       </c>
       <c r="J109" s="58">
-        <f t="shared" si="3"/>
-        <v>1470</v>
+        <f t="shared" ref="J109:N109" si="7">400/0.1</f>
+        <v>4000</v>
       </c>
       <c r="K109" s="58">
-        <f t="shared" si="3"/>
-        <v>1470</v>
+        <f t="shared" si="7"/>
+        <v>4000</v>
       </c>
       <c r="L109" s="58">
-        <f t="shared" si="3"/>
-        <v>1470</v>
+        <f t="shared" si="7"/>
+        <v>4000</v>
       </c>
       <c r="M109" s="58">
-        <f t="shared" si="3"/>
-        <v>1470</v>
+        <f t="shared" si="7"/>
+        <v>4000</v>
       </c>
       <c r="N109" s="58">
-        <f t="shared" si="3"/>
-        <v>1470</v>
+        <f t="shared" si="7"/>
+        <v>4000</v>
       </c>
     </row>
     <row r="110" spans="1:14" x14ac:dyDescent="0.3">
@@ -7962,31 +7963,31 @@
         <v>280800</v>
       </c>
       <c r="H115" s="67">
-        <f t="shared" ref="H115:N115" si="4">0.1 * 3.25 * (60*60*24)</f>
+        <f t="shared" ref="H115:N115" si="8">0.1 * 3.25 * (60*60*24)</f>
         <v>28080</v>
       </c>
       <c r="I115" s="67">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>28080</v>
       </c>
       <c r="J115" s="67">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>28080</v>
       </c>
       <c r="K115" s="67">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>28080</v>
       </c>
       <c r="L115" s="67">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>28080</v>
       </c>
       <c r="M115" s="67">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>28080</v>
       </c>
       <c r="N115" s="67">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>28080</v>
       </c>
     </row>
@@ -8014,31 +8015,31 @@
         <v>1.2847222222222224E-5</v>
       </c>
       <c r="H116" s="67">
-        <f t="shared" ref="H116:N116" si="5">1.11 / 10</f>
+        <f t="shared" ref="H116:N116" si="9">1.11 / 10</f>
         <v>0.11100000000000002</v>
       </c>
       <c r="I116" s="67">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0.11100000000000002</v>
       </c>
       <c r="J116" s="67">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0.11100000000000002</v>
       </c>
       <c r="K116" s="67">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0.11100000000000002</v>
       </c>
       <c r="L116" s="67">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0.11100000000000002</v>
       </c>
       <c r="M116" s="67">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0.11100000000000002</v>
       </c>
       <c r="N116" s="67">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0.11100000000000002</v>
       </c>
     </row>
@@ -8106,35 +8107,35 @@
         <v>430</v>
       </c>
       <c r="G118" s="67">
-        <f t="shared" ref="G118:N118" si="6">5.32 * (60*60*24)</f>
+        <f t="shared" ref="G118:N118" si="10">5.32 * (60*60*24)</f>
         <v>459648</v>
       </c>
       <c r="H118" s="67">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>459648</v>
       </c>
       <c r="I118" s="67">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>459648</v>
       </c>
       <c r="J118" s="67">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>459648</v>
       </c>
       <c r="K118" s="67">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>459648</v>
       </c>
       <c r="L118" s="67">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>459648</v>
       </c>
       <c r="M118" s="67">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>459648</v>
       </c>
       <c r="N118" s="67">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>459648</v>
       </c>
     </row>
@@ -8162,31 +8163,31 @@
         <v>1.2847222222222224E-5</v>
       </c>
       <c r="H119" s="67">
-        <f t="shared" ref="H119:N119" si="7">1.11/8</f>
+        <f t="shared" ref="H119:N119" si="11">1.11/8</f>
         <v>0.13875000000000001</v>
       </c>
       <c r="I119" s="67">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0.13875000000000001</v>
       </c>
       <c r="J119" s="67">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0.13875000000000001</v>
       </c>
       <c r="K119" s="67">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0.13875000000000001</v>
       </c>
       <c r="L119" s="67">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0.13875000000000001</v>
       </c>
       <c r="M119" s="67">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0.13875000000000001</v>
       </c>
       <c r="N119" s="67">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0.13875000000000001</v>
       </c>
     </row>
@@ -8345,31 +8346,31 @@
         <v>2.0833333333333335E-4</v>
       </c>
       <c r="H123" s="78">
-        <f t="shared" ref="H123:N123" si="8">1250*0.000001/6</f>
+        <f t="shared" ref="H123:N123" si="12">1250*0.000001/6</f>
         <v>2.0833333333333335E-4</v>
       </c>
       <c r="I123" s="78">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>2.0833333333333335E-4</v>
       </c>
       <c r="J123" s="78">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>2.0833333333333335E-4</v>
       </c>
       <c r="K123" s="78">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>2.0833333333333335E-4</v>
       </c>
       <c r="L123" s="78">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>2.0833333333333335E-4</v>
       </c>
       <c r="M123" s="78">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>2.0833333333333335E-4</v>
       </c>
       <c r="N123" s="78">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>2.0833333333333335E-4</v>
       </c>
     </row>
@@ -12135,22 +12136,22 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="I209" s="2">
-        <v>2.2000000000000002</v>
+        <v>1.36</v>
       </c>
       <c r="J209" s="2">
-        <v>2.2000000000000002</v>
+        <v>1.36</v>
       </c>
       <c r="K209" s="2">
-        <v>2.2000000000000002</v>
+        <v>1.36</v>
       </c>
       <c r="L209" s="2">
-        <v>2.2000000000000002</v>
+        <v>1.36</v>
       </c>
       <c r="M209" s="2">
-        <v>2.2000000000000002</v>
+        <v>1.36</v>
       </c>
       <c r="N209" s="2">
-        <v>2.2000000000000002</v>
+        <v>1.36</v>
       </c>
     </row>
     <row r="210" spans="1:14" x14ac:dyDescent="0.3">
@@ -12179,22 +12180,22 @@
         <v>-100000</v>
       </c>
       <c r="I210" s="98">
-        <v>-100000</v>
+        <v>-30000</v>
       </c>
       <c r="J210" s="98">
-        <v>-100000</v>
+        <v>-30000</v>
       </c>
       <c r="K210" s="98">
-        <v>-100000</v>
+        <v>-30000</v>
       </c>
       <c r="L210" s="98">
-        <v>-100000</v>
+        <v>-30000</v>
       </c>
       <c r="M210" s="98">
-        <v>-100000</v>
+        <v>-30000</v>
       </c>
       <c r="N210" s="98">
-        <v>-100000</v>
+        <v>-30000</v>
       </c>
     </row>
     <row r="211" spans="1:14" x14ac:dyDescent="0.3">
@@ -12220,32 +12221,32 @@
         <v>-100000</v>
       </c>
       <c r="H211" s="98">
-        <f t="shared" ref="H211:N211" si="9">H210</f>
+        <f t="shared" ref="H211:N211" si="13">H210</f>
         <v>-100000</v>
       </c>
       <c r="I211" s="98">
-        <f t="shared" si="9"/>
-        <v>-100000</v>
+        <f t="shared" si="13"/>
+        <v>-30000</v>
       </c>
       <c r="J211" s="98">
-        <f t="shared" si="9"/>
-        <v>-100000</v>
+        <f t="shared" si="13"/>
+        <v>-30000</v>
       </c>
       <c r="K211" s="98">
-        <f t="shared" si="9"/>
-        <v>-100000</v>
+        <f t="shared" si="13"/>
+        <v>-30000</v>
       </c>
       <c r="L211" s="98">
-        <f t="shared" si="9"/>
-        <v>-100000</v>
+        <f t="shared" si="13"/>
+        <v>-30000</v>
       </c>
       <c r="M211" s="98">
-        <f t="shared" si="9"/>
-        <v>-100000</v>
+        <f t="shared" si="13"/>
+        <v>-30000</v>
       </c>
       <c r="N211" s="98">
-        <f t="shared" si="9"/>
-        <v>-100000</v>
+        <f t="shared" si="13"/>
+        <v>-30000</v>
       </c>
     </row>
     <row r="212" spans="1:14" x14ac:dyDescent="0.3">
@@ -12492,31 +12493,31 @@
         <v>1.2499999999999999E-6</v>
       </c>
       <c r="H217" s="98">
-        <f t="shared" ref="H217:N217" si="10">1250*0.000001/5</f>
+        <f t="shared" ref="H217:N217" si="14">1250*0.000001/5</f>
         <v>2.5000000000000001E-4</v>
       </c>
       <c r="I217" s="98">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>2.5000000000000001E-4</v>
       </c>
       <c r="J217" s="98">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>2.5000000000000001E-4</v>
       </c>
       <c r="K217" s="98">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>2.5000000000000001E-4</v>
       </c>
       <c r="L217" s="98">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>2.5000000000000001E-4</v>
       </c>
       <c r="M217" s="98">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>2.5000000000000001E-4</v>
       </c>
       <c r="N217" s="98">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>2.5000000000000001E-4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
changed water model parametrization for before overlimited evaporation
</commit_message>
<xml_diff>
--- a/simulations/inputs/Scenarios_24_06.xlsx
+++ b/simulations/inputs/Scenarios_24_06.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tigerault\package\Wheat-BRIDGES\Root_BRIDGES\root_cynaps\simulations\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CCE212D-801E-415D-B3F6-8A508692609D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CE666A0-3B02-474A-AC43-C0AEDE34455D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2164" uniqueCount="569">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2173" uniqueCount="572">
   <si>
     <t>input_file</t>
   </si>
@@ -1741,6 +1741,15 @@
   </si>
   <si>
     <t>M3525_47_HN_R2_D1.rsml</t>
+  </si>
+  <si>
+    <t>apoplasmic_water_conductivity</t>
+  </si>
+  <si>
+    <t>m.s-1.Pa-2</t>
+  </si>
+  <si>
+    <t>xylem_cross_area_ratio</t>
   </si>
 </sst>
 </file>
@@ -2933,11 +2942,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:T222"/>
+  <dimension ref="A1:T224"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A192" zoomScale="89" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="P1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="T228" sqref="T228"/>
+    <sheetView tabSelected="1" topLeftCell="A200" zoomScale="89" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="H229" sqref="H229"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16023,27 +16032,27 @@
         <v>1.36</v>
       </c>
       <c r="O209" s="2">
-        <f>1.36+20</f>
+        <f t="shared" ref="O209:T209" si="13">1.36+20</f>
         <v>21.36</v>
       </c>
       <c r="P209" s="2">
-        <f>1.36+20</f>
+        <f t="shared" si="13"/>
         <v>21.36</v>
       </c>
       <c r="Q209" s="2">
-        <f>1.36+20</f>
+        <f t="shared" si="13"/>
         <v>21.36</v>
       </c>
       <c r="R209" s="2">
-        <f>1.36+20</f>
+        <f t="shared" si="13"/>
         <v>21.36</v>
       </c>
       <c r="S209" s="2">
-        <f>1.36+20</f>
+        <f t="shared" si="13"/>
         <v>21.36</v>
       </c>
       <c r="T209" s="2">
-        <f>1.36+20</f>
+        <f t="shared" si="13"/>
         <v>21.36</v>
       </c>
     </row>
@@ -16132,7 +16141,7 @@
         <v>-100000</v>
       </c>
       <c r="H211" s="98">
-        <f t="shared" ref="H211" si="13">H210</f>
+        <f t="shared" ref="H211" si="14">H210</f>
         <v>-100000</v>
       </c>
       <c r="I211" s="98">
@@ -16506,55 +16515,55 @@
         <v>1.2499999999999999E-6</v>
       </c>
       <c r="H217" s="98">
-        <f t="shared" ref="H217:T217" si="14">1250*0.000001/5</f>
+        <f t="shared" ref="H217:T217" si="15">1250*0.000001/5</f>
         <v>2.5000000000000001E-4</v>
       </c>
       <c r="I217" s="98">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>2.5000000000000001E-4</v>
       </c>
       <c r="J217" s="98">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>2.5000000000000001E-4</v>
       </c>
       <c r="K217" s="98">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>2.5000000000000001E-4</v>
       </c>
       <c r="L217" s="98">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>2.5000000000000001E-4</v>
       </c>
       <c r="M217" s="98">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>2.5000000000000001E-4</v>
       </c>
       <c r="N217" s="98">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>2.5000000000000001E-4</v>
       </c>
       <c r="O217" s="98">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>2.5000000000000001E-4</v>
       </c>
       <c r="P217" s="98">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>2.5000000000000001E-4</v>
       </c>
       <c r="Q217" s="98">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>2.5000000000000001E-4</v>
       </c>
       <c r="R217" s="98">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>2.5000000000000001E-4</v>
       </c>
       <c r="S217" s="98">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>2.5000000000000001E-4</v>
       </c>
       <c r="T217" s="98">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>2.5000000000000001E-4</v>
       </c>
     </row>
@@ -16821,9 +16830,7 @@
       <c r="D222" s="2" t="s">
         <v>474</v>
       </c>
-      <c r="E222" s="96" t="s">
-        <v>561</v>
-      </c>
+      <c r="E222" s="96"/>
       <c r="F222" s="96" t="s">
         <v>524</v>
       </c>
@@ -16836,52 +16843,188 @@
         <v>9.9999999999999994E-12</v>
       </c>
       <c r="I222" s="98">
-        <f>0.00000000000001 * 2000</f>
-        <v>1.9999999999999999E-11</v>
+        <f>0.00000000000001*100</f>
+        <v>9.9999999999999998E-13</v>
       </c>
       <c r="J222" s="98">
-        <f t="shared" ref="J222:T222" si="15">0.00000000000001 * 2000</f>
-        <v>1.9999999999999999E-11</v>
+        <f t="shared" ref="J222:T222" si="16">0.00000000000001 * 1000</f>
+        <v>9.9999999999999994E-12</v>
       </c>
       <c r="K222" s="98">
-        <f t="shared" si="15"/>
-        <v>1.9999999999999999E-11</v>
+        <f t="shared" si="16"/>
+        <v>9.9999999999999994E-12</v>
       </c>
       <c r="L222" s="98">
-        <f t="shared" si="15"/>
-        <v>1.9999999999999999E-11</v>
+        <f t="shared" si="16"/>
+        <v>9.9999999999999994E-12</v>
       </c>
       <c r="M222" s="98">
-        <f t="shared" si="15"/>
-        <v>1.9999999999999999E-11</v>
+        <f t="shared" si="16"/>
+        <v>9.9999999999999994E-12</v>
       </c>
       <c r="N222" s="98">
-        <f t="shared" si="15"/>
-        <v>1.9999999999999999E-11</v>
+        <f t="shared" si="16"/>
+        <v>9.9999999999999994E-12</v>
       </c>
       <c r="O222" s="98">
-        <f t="shared" si="15"/>
-        <v>1.9999999999999999E-11</v>
+        <f t="shared" si="16"/>
+        <v>9.9999999999999994E-12</v>
       </c>
       <c r="P222" s="98">
-        <f t="shared" si="15"/>
-        <v>1.9999999999999999E-11</v>
+        <f t="shared" si="16"/>
+        <v>9.9999999999999994E-12</v>
       </c>
       <c r="Q222" s="98">
-        <f t="shared" si="15"/>
-        <v>1.9999999999999999E-11</v>
+        <f t="shared" si="16"/>
+        <v>9.9999999999999994E-12</v>
       </c>
       <c r="R222" s="98">
-        <f t="shared" si="15"/>
-        <v>1.9999999999999999E-11</v>
+        <f t="shared" si="16"/>
+        <v>9.9999999999999994E-12</v>
       </c>
       <c r="S222" s="98">
-        <f t="shared" si="15"/>
-        <v>1.9999999999999999E-11</v>
+        <f t="shared" si="16"/>
+        <v>9.9999999999999994E-12</v>
       </c>
       <c r="T222" s="98">
-        <f t="shared" si="15"/>
-        <v>1.9999999999999999E-11</v>
+        <f t="shared" si="16"/>
+        <v>9.9999999999999994E-12</v>
+      </c>
+    </row>
+    <row r="223" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A223" s="2" t="s">
+        <v>569</v>
+      </c>
+      <c r="B223" s="3" t="s">
+        <v>470</v>
+      </c>
+      <c r="C223" s="2" t="s">
+        <v>528</v>
+      </c>
+      <c r="D223" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="E223" s="96"/>
+      <c r="F223" s="96" t="s">
+        <v>570</v>
+      </c>
+      <c r="G223" s="98">
+        <f>0.00000000000001 * 10000</f>
+        <v>1E-10</v>
+      </c>
+      <c r="H223" s="98">
+        <f>0.00000000000001 * 10000</f>
+        <v>1E-10</v>
+      </c>
+      <c r="I223" s="98">
+        <f>I222*10</f>
+        <v>9.9999999999999994E-12</v>
+      </c>
+      <c r="J223" s="98">
+        <f t="shared" ref="J223:T223" si="17">0.00000000000001 * 10000</f>
+        <v>1E-10</v>
+      </c>
+      <c r="K223" s="98">
+        <f t="shared" si="17"/>
+        <v>1E-10</v>
+      </c>
+      <c r="L223" s="98">
+        <f t="shared" si="17"/>
+        <v>1E-10</v>
+      </c>
+      <c r="M223" s="98">
+        <f t="shared" si="17"/>
+        <v>1E-10</v>
+      </c>
+      <c r="N223" s="98">
+        <f t="shared" si="17"/>
+        <v>1E-10</v>
+      </c>
+      <c r="O223" s="98">
+        <f t="shared" si="17"/>
+        <v>1E-10</v>
+      </c>
+      <c r="P223" s="98">
+        <f t="shared" si="17"/>
+        <v>1E-10</v>
+      </c>
+      <c r="Q223" s="98">
+        <f t="shared" si="17"/>
+        <v>1E-10</v>
+      </c>
+      <c r="R223" s="98">
+        <f t="shared" si="17"/>
+        <v>1E-10</v>
+      </c>
+      <c r="S223" s="98">
+        <f t="shared" si="17"/>
+        <v>1E-10</v>
+      </c>
+      <c r="T223" s="98">
+        <f t="shared" si="17"/>
+        <v>1E-10</v>
+      </c>
+    </row>
+    <row r="224" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A224" s="2" t="s">
+        <v>571</v>
+      </c>
+      <c r="B224" s="3" t="s">
+        <v>470</v>
+      </c>
+      <c r="C224" s="2" t="s">
+        <v>528</v>
+      </c>
+      <c r="D224" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="E224" s="96"/>
+      <c r="F224" s="96" t="s">
+        <v>506</v>
+      </c>
+      <c r="G224" s="98">
+        <f>0.84*(0.36^2)</f>
+        <v>0.10886399999999999</v>
+      </c>
+      <c r="H224" s="98">
+        <f>0.84*(0.36^2)</f>
+        <v>0.10886399999999999</v>
+      </c>
+      <c r="I224" s="98">
+        <v>10</v>
+      </c>
+      <c r="J224" s="98">
+        <v>1</v>
+      </c>
+      <c r="K224" s="98">
+        <v>1</v>
+      </c>
+      <c r="L224" s="98">
+        <v>1</v>
+      </c>
+      <c r="M224" s="98">
+        <v>1</v>
+      </c>
+      <c r="N224" s="98">
+        <v>1</v>
+      </c>
+      <c r="O224" s="98">
+        <v>1</v>
+      </c>
+      <c r="P224" s="98">
+        <v>1</v>
+      </c>
+      <c r="Q224" s="98">
+        <v>1</v>
+      </c>
+      <c r="R224" s="98">
+        <v>1</v>
+      </c>
+      <c r="S224" s="98">
+        <v>1</v>
+      </c>
+      <c r="T224" s="98">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>